<commit_message>
Add activity api & update docu
</commit_message>
<xml_diff>
--- a/TE-Backend.xlsx
+++ b/TE-Backend.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="61">
   <si>
     <t xml:space="preserve">Action</t>
   </si>
@@ -300,6 +300,63 @@
   <si>
     <t xml:space="preserve">section is id</t>
   </si>
+  <si>
+    <t xml:space="preserve">ACTIVITY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List of Activity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/api/activity/viewset/list/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+    "activity_name": "Activity #1",
+    "chapter": 3
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/api/activity/viewset/list/&lt;int:pk&gt;/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">get specific activity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set prof activity date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/api/activity/viewset/prof_activity/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+    "activity": 1,
+    "section": 5,
+    "start": "2020-12-16",
+    "end": "2020-12-20",
+    "remarks": false
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List of Activity (Prof)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+        "id": 1,
+        "activity": 1,
+        "activity_name": "Activity #1",
+        "section": 5,
+        "section_code": "CEIT--03-1001E",
+        "start": "2020-11-16",
+        "end": "2020-11-20",
+        "remarks": false
+    }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/api/activity/viewset/prof_activity/&lt;int:pk&gt;/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">get specific activity (prof)</t>
+  </si>
 </sst>
 </file>
 
@@ -446,8 +503,8 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -527,18 +584,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="29.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="29.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="32.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="28.62"/>
   </cols>
   <sheetData>
@@ -720,14 +777,65 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="40.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C16" s="0" t="s">
+        <v>52</v>
+      </c>
       <c r="D16" s="11"/>
+      <c r="E16" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C19" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>60</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="D11:D12"/>
+    <mergeCell ref="D15:D16"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId1" display="{&#10;   “email”: “sample@test.com”&#10;}"/>

</xml_diff>

<commit_message>
Add question and choices
</commit_message>
<xml_diff>
--- a/TE-Backend.xlsx
+++ b/TE-Backend.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="66">
   <si>
     <t xml:space="preserve">Action</t>
   </si>
@@ -357,6 +357,41 @@
   <si>
     <t xml:space="preserve">get specific activity (prof)</t>
   </si>
+  <si>
+    <t xml:space="preserve">QUESTION &amp; ANSWER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">list view</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/api/question/list/&lt;activity&gt;/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+        "number": 1,
+        "id": 1,
+        "q_type": "IDENT",
+        "question_name": "This is a question #1",
+        "choices": []
+    },
+    {
+        "number": 2,
+        "id": 2,
+        "q_type": "MULT",
+        "question_name": "This is a question multiple #2",
+        "choices": [
+            {
+                "description": "A. sample"
+            },
+            {
+                "description": "B. sample"
+            }
+        ]
+    }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">get only method</t>
+  </si>
 </sst>
 </file>
 
@@ -458,7 +493,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -501,10 +536,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -584,13 +615,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.11"/>
@@ -787,7 +818,7 @@
       <c r="C15" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="8" t="s">
         <v>51</v>
       </c>
     </row>
@@ -795,7 +826,7 @@
       <c r="C16" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="D16" s="11"/>
+      <c r="D16" s="8"/>
       <c r="E16" s="0" t="s">
         <v>53</v>
       </c>
@@ -828,6 +859,23 @@
       </c>
       <c r="E19" s="0" t="s">
         <v>60</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="236.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add student submit answer
</commit_message>
<xml_diff>
--- a/TE-Backend.xlsx
+++ b/TE-Backend.xlsx
@@ -403,9 +403,8 @@
   </si>
   <si>
     <t xml:space="preserve">{
-   “user”: 1,
    “question”: 2,
-   “description”: “TEXT”
+   “answer”: “TEXT”
 }</t>
   </si>
   <si>
@@ -637,11 +636,11 @@
   </sheetPr>
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E32" activeCellId="0" sqref="E32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.11"/>

</xml_diff>

<commit_message>
Add summary view and update score
</commit_message>
<xml_diff>
--- a/TE-Backend.xlsx
+++ b/TE-Backend.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="86">
   <si>
     <t xml:space="preserve">Action</t>
   </si>
@@ -444,6 +444,100 @@
     <t xml:space="preserve">after submit automatic activity
 Remarks equal to true</t>
   </si>
+  <si>
+    <t xml:space="preserve">View Summary Answer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Summary</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">http://127.0.0.1:8000/api/student/summary/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;int:activity&gt;/</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">[
+    {
+        "id": 25,
+        "question": 34,
+        "q_type": "IDENT",
+        "qestion_name": "1224",
+        "student": 16,
+        "answer": "4C8",
+        "table_image": null,
+        "code_file": null
+    },
+    {
+        "id": 26,
+        "question": 33,
+        "q_type": "IDENT",
+        "qestion_name": "1024",
+        "student": 16,
+        "answer": "400",
+        "table_image": null,
+        "code_file": null
+    },
+    {
+        "id": 27,
+        "question": 33,
+        "q_type": "IDENT",
+        "qestion_name": "1024",
+        "student": 16,
+        "answer": null,
+        "table_image": "/media/table_images/Screenshot_from_2020-11-22_01-02-01.png",
+        "code_file": null
+    }
+]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Submit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[
+    {
+        "id": 25,
+        "question": 34,
+        "q_type": "IDENT",
+        "student": 16,
+        "answer": "4C8",
+        "assesment": {
+            "score": 3
+        }
+    },
+    {
+        "id": 26,
+        "question": 33,
+        "q_type": "IDENT",
+        "student": 16,
+        "answer": "400",
+        "assesment": {
+            "score": 1
+        }
+    }
+]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POST</t>
+  </si>
 </sst>
 </file>
 
@@ -679,13 +773,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A23" colorId="64" zoomScale="43" zoomScaleNormal="43" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J26" activeCellId="0" sqref="J26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.11"/>
@@ -981,12 +1075,48 @@
         <v>77</v>
       </c>
     </row>
+    <row r="25" customFormat="false" ht="357.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="2"/>
+    </row>
+    <row r="27" customFormat="false" ht="246.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="D15:D16"/>
+    <mergeCell ref="A25:A27"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId1" display="{&#10;   “email”: “sample@test.com”&#10;}"/>
@@ -996,7 +1126,9 @@
     <hyperlink ref="C18" r:id="rId5" display="http://127.0.0.1:8000/api/activity/viewset/&lt;int:activity_type&gt;/&lt;int:pk&gt;/prof_activi"/>
     <hyperlink ref="C19" r:id="rId6" display="http://127.0.0.1:8000/api/activity/viewset/&lt;int:activity_type&gt;/&lt;int:pk&gt;/prof_activity"/>
     <hyperlink ref="C20" r:id="rId7" display="http://127.0.0.1:8000/api/activity/type/"/>
-    <hyperlink ref="C21" r:id="rId8" display="http://127.0.0.1:8000/api/activity/student/"/>
+    <hyperlink ref="C21" r:id="rId8" display="http://127.0.0.1:8000/api/activity/student/&lt;int:activity_type&gt;/"/>
+    <hyperlink ref="C25" r:id="rId9" display="http://127.0.0.1:8000/api/student/summary/"/>
+    <hyperlink ref="C27" r:id="rId10" display="http://127.0.0.1:8000/api/student/summary/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Add filter records by section
</commit_message>
<xml_diff>
--- a/TE-Backend.xlsx
+++ b/TE-Backend.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="94">
   <si>
     <t xml:space="preserve">Action</t>
   </si>
@@ -451,25 +451,7 @@
     <t xml:space="preserve">Summary</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">http://127.0.0.1:8000/api/student/summary/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;int:activity&gt;/</t>
-    </r>
+    <t xml:space="preserve">http://127.0.0.1:8000/api/student/summary/&lt;int:activity&gt;/</t>
   </si>
   <si>
     <t xml:space="preserve">[
@@ -537,6 +519,52 @@
   </si>
   <si>
     <t xml:space="preserve">POST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assesnebt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Records</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://127.0.0.1:8000/api/assesment/list/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[
+    {
+        "university_id": "2020-100002",
+        "full_name": "123 123 123",
+        "assesment": []
+    },
+    {
+        "university_id": "2015-105861",
+        "full_name": "Parreno Jhon Rhay L.",
+        "assesment": [
+            {
+                "activity": 16,
+                "score": 2.0,
+                "date_taken": "2020-11-21"
+            }
+        ]
+    },
+    {
+        "university_id": "2020-100003",
+        "full_name": "123 123 123",
+        "assesment": []
+    }
+]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">View all</t>
+  </si>
+  <si>
+    <t xml:space="preserve">filter records</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://127.0.0.1:8000/api/assesment/list/filter/1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">filter by section id</t>
   </si>
 </sst>
 </file>
@@ -773,13 +801,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A23" colorId="64" zoomScale="43" zoomScaleNormal="43" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J26" activeCellId="0" sqref="J26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A26" colorId="64" zoomScale="43" zoomScaleNormal="43" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L30" activeCellId="0" sqref="L30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.11"/>
@@ -1076,7 +1104,7 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="357.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="9" t="s">
         <v>78</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -1093,10 +1121,10 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="2"/>
+      <c r="A26" s="9"/>
     </row>
     <row r="27" customFormat="false" ht="246.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="2"/>
+      <c r="A27" s="9"/>
       <c r="B27" s="2" t="s">
         <v>83</v>
       </c>
@@ -1108,6 +1136,34 @@
       </c>
       <c r="F27" s="2" t="s">
         <v>85</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="256.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1127,8 +1183,10 @@
     <hyperlink ref="C19" r:id="rId6" display="http://127.0.0.1:8000/api/activity/viewset/&lt;int:activity_type&gt;/&lt;int:pk&gt;/prof_activity"/>
     <hyperlink ref="C20" r:id="rId7" display="http://127.0.0.1:8000/api/activity/type/"/>
     <hyperlink ref="C21" r:id="rId8" display="http://127.0.0.1:8000/api/activity/student/&lt;int:activity_type&gt;/"/>
-    <hyperlink ref="C25" r:id="rId9" display="http://127.0.0.1:8000/api/student/summary/"/>
-    <hyperlink ref="C27" r:id="rId10" display="http://127.0.0.1:8000/api/student/summary/"/>
+    <hyperlink ref="C25" r:id="rId9" display="http://127.0.0.1:8000/api/student/summary/&lt;int:activity&gt;/"/>
+    <hyperlink ref="C27" r:id="rId10" display="http://127.0.0.1:8000/api/student/summary/&lt;int:activity&gt;/"/>
+    <hyperlink ref="C30" r:id="rId11" display="http://127.0.0.1:8000/api/assesment/list/"/>
+    <hyperlink ref="C32" r:id="rId12" display="http://127.0.0.1:8000/api/assesment/list/filter/1"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Add filter by section and activity for summary
</commit_message>
<xml_diff>
--- a/TE-Backend.xlsx
+++ b/TE-Backend.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="91">
   <si>
     <t xml:space="preserve">Action</t>
   </si>
@@ -451,25 +451,7 @@
     <t xml:space="preserve">Summary</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">http://127.0.0.1:8000/api/student/summary/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;int:activity&gt;/</t>
-    </r>
+    <t xml:space="preserve">http://127.0.0.1:8000/api/student/summary/&lt;int:activity&gt;/</t>
   </si>
   <si>
     <t xml:space="preserve">[
@@ -512,6 +494,9 @@
     <t xml:space="preserve">Submit</t>
   </si>
   <si>
+    <t xml:space="preserve">http://127.0.0.1:8000/api/student/summary/&lt;int:activity&gt;/update</t>
+  </si>
+  <si>
     <t xml:space="preserve">[
     {
         "id": 25,
@@ -538,6 +523,53 @@
   <si>
     <t xml:space="preserve">POST</t>
   </si>
+  <si>
+    <t xml:space="preserve">Summary Section Activity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://127.0.0.1:8000/api/student/summary/1/16/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[
+    {
+        "full_name": "Parreno Jhon Rhay L.",
+        "student_number": "2015-105861",
+        "submitsummary": [
+            {
+                "id": 40,
+                "question": 35,
+                "q_type": "CODE",
+                "qestion_name": "Create a C++/JAVA program that converts BINARY to HEXADECIMAL",
+                "student": 13,
+                "answer": null,
+                "table_image": null,
+                "code_file": "http://127.0.0.1:8000/media/code/requirements.txt"
+            }
+        ]
+    }
+]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;int:section&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/&lt;int:activity/</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -546,7 +578,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -596,6 +628,13 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -639,7 +678,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -694,6 +733,10 @@
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -773,13 +816,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A23" colorId="64" zoomScale="43" zoomScaleNormal="43" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J26" activeCellId="0" sqref="J26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A26" colorId="64" zoomScale="43" zoomScaleNormal="43" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N30" activeCellId="0" sqref="N30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.11"/>
@@ -1076,7 +1119,7 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="357.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="9" t="s">
         <v>78</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -1093,21 +1136,35 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="2"/>
+      <c r="A26" s="9"/>
     </row>
     <row r="27" customFormat="false" ht="246.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="2"/>
+      <c r="A27" s="9"/>
       <c r="B27" s="2" t="s">
         <v>83</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="201.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1127,8 +1184,9 @@
     <hyperlink ref="C19" r:id="rId6" display="http://127.0.0.1:8000/api/activity/viewset/&lt;int:activity_type&gt;/&lt;int:pk&gt;/prof_activity"/>
     <hyperlink ref="C20" r:id="rId7" display="http://127.0.0.1:8000/api/activity/type/"/>
     <hyperlink ref="C21" r:id="rId8" display="http://127.0.0.1:8000/api/activity/student/&lt;int:activity_type&gt;/"/>
-    <hyperlink ref="C25" r:id="rId9" display="http://127.0.0.1:8000/api/student/summary/"/>
-    <hyperlink ref="C27" r:id="rId10" display="http://127.0.0.1:8000/api/student/summary/"/>
+    <hyperlink ref="C25" r:id="rId9" display="http://127.0.0.1:8000/api/student/summary/&lt;int:activity&gt;/"/>
+    <hyperlink ref="C27" r:id="rId10" display="http://127.0.0.1:8000/api/student/summary/&lt;int:activity&gt;/"/>
+    <hyperlink ref="C29" r:id="rId11" display="http://127.0.0.1:8000/api/student/summary/1/16/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Fix filter of students
</commit_message>
<xml_diff>
--- a/TE-Backend.xlsx
+++ b/TE-Backend.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="96">
   <si>
     <t xml:space="preserve">Action</t>
   </si>
@@ -558,6 +558,47 @@
       <t xml:space="preserve">/&lt;int:activity/</t>
     </r>
   </si>
+  <si>
+    <t xml:space="preserve">Assesment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">update score of specific student</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">http://127.0.0.1:8000/api/student/update/3/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">18/</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">[
+    {
+        "question": 35,
+        "q_type": "CODE",
+        "assesment": {
+            "score": 123
+        }
+    }
+]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;int:student_id&gt;/&lt;int:activity&gt;/</t>
+  </si>
 </sst>
 </file>
 
@@ -804,13 +845,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A26" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27:C28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C32" activeCellId="0" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.11"/>
@@ -1153,6 +1194,23 @@
       </c>
       <c r="E29" s="14" t="s">
         <v>90</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1175,6 +1233,7 @@
     <hyperlink ref="C25" r:id="rId9" display="http://127.0.0.1:8000/api/student/summary/&lt;int:activity&gt;/"/>
     <hyperlink ref="C27" r:id="rId10" display="http://127.0.0.1:8000/api/student/summary/&lt;int:activity&gt;/update"/>
     <hyperlink ref="C29" r:id="rId11" display="http://127.0.0.1:8000/api/student/summary/1/16/"/>
+    <hyperlink ref="C32" r:id="rId12" display="http://127.0.0.1:8000/api/student/update/3/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Add student list per section
</commit_message>
<xml_diff>
--- a/TE-Backend.xlsx
+++ b/TE-Backend.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="101">
   <si>
     <t xml:space="preserve">Action</t>
   </si>
@@ -565,25 +565,7 @@
     <t xml:space="preserve">update score of specific student</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">http://127.0.0.1:8000/api/student/update/3/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">18/</t>
-    </r>
+    <t xml:space="preserve">http://127.0.0.1:8000/api/student/update/3/18/</t>
   </si>
   <si>
     <t xml:space="preserve">[
@@ -598,6 +580,50 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;int:student_id&gt;/&lt;int:activity&gt;/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">View prof student list per section</t>
+  </si>
+  <si>
+    <t xml:space="preserve">student list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://127.0.0.1:8000/api/student/section/list/1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[
+    {
+        "student_id": "5",
+        "full_name": "123 123 123",
+        "student_number": "2020-100003"
+    },
+    {
+        "student_id": "13",
+        "full_name": "Parreno Jhon Rhay L.",
+        "student_number": "2015-105861"
+    }
+]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;int:section</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&gt;/</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -845,13 +871,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C32" activeCellId="0" sqref="C32"/>
+      <selection pane="topLeft" activeCell="D39" activeCellId="0" sqref="D39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.11"/>
@@ -1211,6 +1237,23 @@
       </c>
       <c r="E32" s="0" t="s">
         <v>95</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="E35" s="14" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1233,7 +1276,8 @@
     <hyperlink ref="C25" r:id="rId9" display="http://127.0.0.1:8000/api/student/summary/&lt;int:activity&gt;/"/>
     <hyperlink ref="C27" r:id="rId10" display="http://127.0.0.1:8000/api/student/summary/&lt;int:activity&gt;/update"/>
     <hyperlink ref="C29" r:id="rId11" display="http://127.0.0.1:8000/api/student/summary/1/16/"/>
-    <hyperlink ref="C32" r:id="rId12" display="http://127.0.0.1:8000/api/student/update/3/"/>
+    <hyperlink ref="C32" r:id="rId12" display="http://127.0.0.1:8000/api/student/update/3/18/"/>
+    <hyperlink ref="C35" r:id="rId13" display="http://127.0.0.1:8000/api/student/section/list/1"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>